<commit_message>
Make minor changes to the data files, such as removing the NodeOrder column since it is no longer needed
</commit_message>
<xml_diff>
--- a/data-files/Poudre_PointFlow_Dataset.xlsx
+++ b/data-files/Poudre_PointFlow_Dataset.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kms\owf-lib-viz-streamflow-heatmaps\Heatmap\Poudre-Daily-Streamflow\data-files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kms\owf-model-pointflow-co-poudre\data-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3555,7 +3555,7 @@
   <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>